<commit_message>
Replace zoneLong and zoneLat with zoneNumber in schemas, update Yelp request
</commit_message>
<xml_diff>
--- a/server/establishments/categories.xlsx
+++ b/server/establishments/categories.xlsx
@@ -2190,7 +2190,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G290"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>